<commit_message>
added tree size 4192
</commit_message>
<xml_diff>
--- a/Docs/octree_stats.xlsx
+++ b/Docs/octree_stats.xlsx
@@ -53,8 +53,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="#,##0.00&quot;s&quot;"/>
-    <numFmt numFmtId="171" formatCode="#,##0.0&quot; MB&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00&quot;s&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0&quot; MB&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -96,13 +96,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -117,14 +117,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -133,15 +133,14 @@
   </cellStyles>
   <dxfs count="20">
     <dxf>
-      <numFmt numFmtId="171" formatCode="#,##0.0&quot; MB&quot;"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="#,##0.0&quot; MB&quot;"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="#,##0.0&quot; MB&quot;"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.0&quot; MB&quot;"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00&quot;s&quot;"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -152,50 +151,51 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.0&quot; MB&quot;"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.0&quot; MB&quot;"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00&quot;s&quot;"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00&quot;s&quot;"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00&quot;s&quot;"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00&quot;s&quot;"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00&quot;s&quot;"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00&quot;s&quot;"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00&quot;s&quot;"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -324,6 +324,9 @@
                 <c:pt idx="3">
                   <c:v>1669.92</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>14174.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -388,6 +391,9 @@
                 <c:pt idx="3">
                   <c:v>262.90800000000002</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>1118.9100000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -452,6 +458,9 @@
                 <c:pt idx="3">
                   <c:v>94.251000000000005</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>394.29599999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -467,11 +476,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="600385024"/>
-        <c:axId val="597676544"/>
+        <c:axId val="103987200"/>
+        <c:axId val="101128384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="600385024"/>
+        <c:axId val="103987200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -500,7 +509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="597676544"/>
+        <c:crossAx val="101128384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -508,7 +517,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="597676544"/>
+        <c:axId val="101128384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,7 +528,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="600385024"/>
+        <c:crossAx val="103987200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -639,6 +648,9 @@
                 <c:pt idx="3">
                   <c:v>2112</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>8000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -703,6 +715,9 @@
                 <c:pt idx="3">
                   <c:v>930</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>3721</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -718,11 +733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="651659264"/>
-        <c:axId val="599626816"/>
+        <c:axId val="114745344"/>
+        <c:axId val="114057792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="651659264"/>
+        <c:axId val="114745344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +766,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="599626816"/>
+        <c:crossAx val="114057792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="599626816"/>
+        <c:axId val="114057792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,7 +785,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="651659264"/>
+        <c:crossAx val="114745344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -858,20 +873,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="A1:I6" headerRowDxfId="19" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabelle6" displayName="Tabelle6" ref="A1:I6" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:I6"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="PC" totalsRowLabel="Ergebnis" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Treesize" dataDxfId="18" totalsRowDxfId="7"/>
-    <tableColumn id="3" name="Generating" dataDxfId="17" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="Saving" dataDxfId="16" totalsRowDxfId="9"/>
-    <tableColumn id="5" name="Loading" dataDxfId="15" totalsRowDxfId="10"/>
-    <tableColumn id="6" name="RAM used" dataDxfId="0" totalsRowDxfId="11"/>
-    <tableColumn id="7" name="RAM reserved" dataDxfId="2" totalsRowDxfId="12"/>
-    <tableColumn id="8" name="RAM Usage" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="13">
+    <tableColumn id="1" name="PC" totalsRowLabel="Ergebnis" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="2" name="Treesize" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="3" name="Generating" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="4" name="Saving" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="5" name="Loading" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="6" name="RAM used" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="7" name="RAM reserved" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="8" name="RAM Usage" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2">
       <calculatedColumnFormula>Tabelle6[[#This Row],[RAM used]]/Tabelle6[[#This Row],[RAM reserved]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Filesize" dataDxfId="1" totalsRowDxfId="5"/>
+    <tableColumn id="9" name="Filesize" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1167,7 +1182,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,16 +1353,28 @@
       <c r="B6" s="8">
         <v>4096</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="11" t="e">
+      <c r="C6" s="5">
+        <v>14174.5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1118.9100000000001</v>
+      </c>
+      <c r="E6" s="5">
+        <v>394.29599999999999</v>
+      </c>
+      <c r="F6" s="14">
+        <v>3721</v>
+      </c>
+      <c r="G6" s="14">
+        <v>8000</v>
+      </c>
+      <c r="H6" s="11">
         <f>Tabelle6[[#This Row],[RAM used]]/Tabelle6[[#This Row],[RAM reserved]]</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I6" s="14"/>
+        <v>0.46512500000000001</v>
+      </c>
+      <c r="I6" s="14">
+        <v>676</v>
+      </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>

</xml_diff>